<commit_message>
second round touch gfx
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="54">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -147,6 +147,36 @@
   </si>
   <si>
     <t xml:space="preserve">Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEXT ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPOGRAPHY NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIGNMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIRECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello</t>
   </si>
 </sst>
 </file>
@@ -1596,32 +1626,39 @@
       </c>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>12</v>
+      <c r="F3" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="15" customHeight="1"/>
+    <row r="4" spans="2:10" ht="15" customHeight="1">
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="5" spans="2:10" ht="15" customHeight="1"/>
     <row r="6" spans="2:10"/>
     <row r="7" spans="2:10"/>

</xml_diff>